<commit_message>
[updated] update request list
</commit_message>
<xml_diff>
--- a/request list.xlsx
+++ b/request list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>실행 시 실행여부 확인하는 메시지 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>프로그램 실행 중일때도 로그파일 수집 가능하게하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>문자입력에 대한 예외처리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -86,6 +82,18 @@
   </si>
   <si>
     <t>로그파일 수집 로직</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVR OEM버전 로그수집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로그램 실행 중일때도 로그파일 수집할 수 있는 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVR OEM버전에서도 로그 수집할 수 있는 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -352,9 +360,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -368,17 +373,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -388,9 +387,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -407,6 +403,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -720,96 +728,96 @@
     <col min="2" max="2" width="9" style="2"/>
     <col min="3" max="3" width="15.25" customWidth="1"/>
     <col min="4" max="4" width="46.625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="2:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="17">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="24"/>
+      <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="22">
+      <c r="B8" s="18">
         <v>4</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="26"/>
+      <c r="F8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -828,93 +836,97 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.25" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
     <col min="4" max="4" width="46.625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="33.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="2:6" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" s="4" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="26"/>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="17">
-        <v>2</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="17">
-        <v>3</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+      <c r="D7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="22">
+      <c r="B8" s="18">
         <v>4</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>